<commit_message>
added boxplot analysis of QPE
</commit_message>
<xml_diff>
--- a/Paper Figures/Performance Analysis/QPEDataClean.xlsx
+++ b/Paper Figures/Performance Analysis/QPEDataClean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Quantum-Algorithm-Implementations\Paper Figures\Performance Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Quantum-Algorithm-Implementations\Paper Figures\Performance Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D50D8029-633C-4F06-BE1F-EE27AB79AFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B161DA08-61FC-496B-8B19-6AF2FAD999F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{605C24A8-B075-45C2-A3BC-18E55505DDC2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{605C24A8-B075-45C2-A3BC-18E55505DDC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,13 +42,13 @@
     <t>Cirq</t>
   </si>
   <si>
-    <t>Q# loop in Q#</t>
-  </si>
-  <si>
     <t>Q# no Postpro</t>
   </si>
   <si>
     <t>Q# with Postpro</t>
+  </si>
+  <si>
+    <t>Q# loop inside of Q#</t>
   </si>
 </sst>
 </file>
@@ -419,19 +419,19 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="A1:E11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,16 +439,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>113</v>
       </c>
@@ -465,7 +465,7 @@
         <v>41814</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>108</v>
       </c>
@@ -482,7 +482,7 @@
         <v>36811</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>102</v>
       </c>
@@ -499,7 +499,7 @@
         <v>34006</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>105</v>
       </c>
@@ -516,7 +516,7 @@
         <v>34279</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>106</v>
       </c>
@@ -533,7 +533,7 @@
         <v>33690</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -550,7 +550,7 @@
         <v>36302</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>103</v>
       </c>
@@ -567,7 +567,7 @@
         <v>36416</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>102</v>
       </c>
@@ -584,7 +584,7 @@
         <v>34511</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>102</v>
       </c>
@@ -601,7 +601,7 @@
         <v>33723</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>102</v>
       </c>

</xml_diff>